<commit_message>
[Data gathering] Added the group resulsts in a .xlsx
</commit_message>
<xml_diff>
--- a/manual/group_results/Comparative_Analysis_of_IPs.xlsx
+++ b/manual/group_results/Comparative_Analysis_of_IPs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jonas\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/attrup/Desktop/University/Master/Cyber1/Project - Let Me Out/let-me-out/manual/group_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC4E0FAC-FA0F-416F-ACB3-6913A2566058}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF05FF32-517F-C346-B821-F162DAE02FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D0933BE7-A6D3-5840-9958-232435785B00}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{D0933BE7-A6D3-5840-9958-232435785B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1082,7 +1082,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
-    <numFmt numFmtId="173" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="165" formatCode="dd\-mm\-yyyy"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -1341,7 +1341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1366,6 +1366,21 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
@@ -1374,17 +1389,17 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFDDDDDD"/>
-      </top>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -1397,98 +1412,96 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="4" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="6" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="4" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="7" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="10" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="2" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="2" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="4" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="2" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="5" fillId="11" borderId="2" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="2" xfId="4" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="15" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="2" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="6" fillId="14" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="10" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="14" fontId="5" fillId="11" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="4" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="4" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" xfId="5" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="3" xfId="4" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="24" fillId="14" borderId="0" xfId="4" applyFont="1" applyFill="1"/>
-    <xf numFmtId="173" fontId="6" fillId="14" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Bemærk!" xfId="2" builtinId="10"/>
-    <cellStyle name="God" xfId="1" builtinId="26"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Link 2" xfId="5" xr:uid="{466EE1D8-4108-4681-842C-0F992AF2DB82}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="3" xr:uid="{AAED286B-8202-4E38-B932-A6B7EDCDA0DA}"/>
     <cellStyle name="Normal 3" xfId="4" xr:uid="{8A03B0C8-2B43-479F-970E-FE9137C96AA7}"/>
+    <cellStyle name="Note" xfId="2" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1510,7 +1523,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1809,33 +1822,33 @@
   <dimension ref="A1:S90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+      <selection activeCell="C71" sqref="C71:C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="2" max="2" width="53.125" customWidth="1"/>
+    <col min="2" max="2" width="53.1640625" customWidth="1"/>
     <col min="3" max="3" width="52" customWidth="1"/>
     <col min="4" max="4" width="61" customWidth="1"/>
-    <col min="5" max="5" width="42.875" customWidth="1"/>
-    <col min="6" max="6" width="28.375" customWidth="1"/>
-    <col min="7" max="7" width="33.375" customWidth="1"/>
-    <col min="8" max="8" width="41.375" customWidth="1"/>
-    <col min="9" max="9" width="32.625" customWidth="1"/>
-    <col min="10" max="10" width="46.875" customWidth="1"/>
+    <col min="5" max="5" width="42.83203125" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="33.33203125" customWidth="1"/>
+    <col min="8" max="8" width="41.33203125" customWidth="1"/>
+    <col min="9" max="9" width="32.6640625" customWidth="1"/>
+    <col min="10" max="10" width="46.83203125" customWidth="1"/>
     <col min="11" max="11" width="97.5" customWidth="1"/>
     <col min="12" max="12" width="43" customWidth="1"/>
-    <col min="13" max="13" width="67.625" customWidth="1"/>
-    <col min="14" max="14" width="62.875" customWidth="1"/>
-    <col min="15" max="15" width="54.375" customWidth="1"/>
-    <col min="16" max="16" width="110.25" customWidth="1"/>
+    <col min="13" max="13" width="67.6640625" customWidth="1"/>
+    <col min="14" max="14" width="62.83203125" customWidth="1"/>
+    <col min="15" max="15" width="54.33203125" customWidth="1"/>
+    <col min="16" max="16" width="110.1640625" customWidth="1"/>
     <col min="17" max="17" width="63.5" customWidth="1"/>
     <col min="18" max="18" width="92.5" customWidth="1"/>
-    <col min="19" max="19" width="104.625" customWidth="1"/>
+    <col min="19" max="19" width="104.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="31.5">
+    <row r="1" spans="1:19" ht="31">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1894,1574 +1907,1574 @@
         <v>288</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="31.5">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:19" ht="31">
+      <c r="A2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="5" t="s">
+      <c r="I2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="5" t="s">
+      <c r="K2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="5" t="s">
+      <c r="M2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="O2" s="6">
+      <c r="O2" s="3">
         <v>44980</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" s="5" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="R2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="25" t="s">
+      <c r="S2" s="4" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:19">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="G3" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="H3" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M3" s="8" t="s">
+      <c r="M3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="N3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="O3" s="9">
+      <c r="N3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="7">
         <v>42130</v>
       </c>
-      <c r="P3" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="8" t="s">
+      <c r="P3" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="S3" s="4"/>
+      <c r="S3" s="8"/>
     </row>
     <row r="4" spans="1:19">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="G4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="L4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="M4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="N4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q4" s="5" t="s">
+      <c r="N4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q4" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="R4" s="5" t="s">
+      <c r="R4" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="S4" s="4"/>
-    </row>
-    <row r="5" spans="1:19" ht="31.5">
-      <c r="A5" s="10" t="s">
+      <c r="S4" s="8"/>
+    </row>
+    <row r="5" spans="1:19" ht="31">
+      <c r="A5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E5" s="10" t="s">
+      <c r="E5" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="F5" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="I5" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="J5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="K5" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="L5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="M5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="N5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="O5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q5" s="10" t="s">
+      <c r="O5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P5" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q5" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R5" s="10" t="s">
+      <c r="R5" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="S5" s="24" t="s">
+      <c r="S5" s="10" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="30">
-      <c r="A6" s="10" t="s">
+    <row r="6" spans="1:19" ht="32">
+      <c r="A6" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="C6" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="E6" s="10" t="s">
+      <c r="E6" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F6" s="10" t="s">
+      <c r="F6" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G6" s="10" t="s">
+      <c r="G6" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="H6" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="I6" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="J6" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="L6" s="10" t="s">
+      <c r="L6" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="M6" s="10" t="s">
+      <c r="M6" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="N6" s="10" t="s">
+      <c r="N6" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="O6" s="10">
+      <c r="O6" s="9">
         <v>45262</v>
       </c>
-      <c r="P6" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q6" s="10" t="s">
+      <c r="P6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q6" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R6" s="10" t="s">
+      <c r="R6" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S6" s="11"/>
     </row>
-    <row r="7" spans="1:19" ht="30">
-      <c r="A7" s="10" t="s">
+    <row r="7" spans="1:19" ht="32">
+      <c r="A7" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E7" s="10" t="s">
+      <c r="E7" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F7" s="10" t="s">
+      <c r="F7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G7" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="H7" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="I7" s="9" t="s">
         <v>277</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="K7" s="10" t="s">
+      <c r="K7" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L7" s="10" t="s">
+      <c r="L7" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="M7" s="10" t="s">
+      <c r="M7" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="N7" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="O7" s="10">
+      <c r="O7" s="9">
         <v>43381</v>
       </c>
-      <c r="P7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q7" s="10" t="s">
+      <c r="P7" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q7" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="R7" s="10" t="s">
+      <c r="R7" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S7" s="11"/>
     </row>
     <row r="8" spans="1:19">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="C8" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E8" s="10" t="s">
+      <c r="E8" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="G8" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="H8" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="I8" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="J8" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="K8" s="10" t="s">
+      <c r="K8" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="L8" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="M8" s="10" t="s">
+      <c r="M8" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="N8" s="10" t="s">
+      <c r="N8" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="O8" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="P8" s="10" t="s">
+      <c r="O8" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P8" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="Q8" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R8" s="10" t="s">
+      <c r="R8" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S8" s="11"/>
     </row>
-    <row r="9" spans="1:19" ht="105">
-      <c r="A9" s="10" t="s">
+    <row r="9" spans="1:19" ht="112">
+      <c r="A9" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="E9" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="F9" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="10" t="s">
+      <c r="G9" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="H9" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="I9" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="L9" s="10" t="s">
+      <c r="L9" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="M9" s="10" t="s">
+      <c r="M9" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="N9" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="O9" s="10">
+      <c r="O9" s="9">
         <v>44769</v>
       </c>
-      <c r="P9" s="10" t="s">
+      <c r="P9" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="Q9" s="10" t="s">
+      <c r="Q9" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="R9" s="10" t="s">
+      <c r="R9" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S9" s="11"/>
     </row>
-    <row r="10" spans="1:19" ht="105">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:19" ht="112">
+      <c r="A10" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E10" s="10" t="s">
+      <c r="E10" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F10" s="10" t="s">
+      <c r="F10" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G10" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="H10" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="I10" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="L10" s="10" t="s">
+      <c r="L10" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="M10" s="10" t="s">
+      <c r="M10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="N10" s="10" t="s">
+      <c r="N10" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="O10" s="10">
+      <c r="O10" s="9">
         <v>44641</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="P10" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="Q10" s="10" t="s">
+      <c r="Q10" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R10" s="10" t="s">
+      <c r="R10" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S10" s="11"/>
     </row>
-    <row r="11" spans="1:19" ht="60">
-      <c r="A11" s="10" t="s">
+    <row r="11" spans="1:19" ht="64">
+      <c r="A11" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="C11" s="10" t="s">
+      <c r="C11" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E11" s="10" t="s">
+      <c r="E11" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G11" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="H11" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="I11" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="K11" s="10" t="s">
+      <c r="K11" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="L11" s="10" t="s">
+      <c r="L11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="M11" s="10" t="s">
+      <c r="M11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="N11" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="O11" s="10">
+      <c r="O11" s="9">
         <v>44444</v>
       </c>
-      <c r="P11" s="10" t="s">
+      <c r="P11" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="Q11" s="10" t="s">
+      <c r="Q11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R11" s="10" t="s">
+      <c r="R11" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S11" s="11"/>
     </row>
-    <row r="12" spans="1:19" ht="45">
-      <c r="A12" s="10" t="s">
+    <row r="12" spans="1:19" ht="48">
+      <c r="A12" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E12" s="10" t="s">
+      <c r="E12" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F12" s="10" t="s">
+      <c r="F12" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G12" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="H12" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="I12" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="K12" s="10" t="s">
+      <c r="K12" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="L12" s="10" t="s">
+      <c r="L12" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="M12" s="10" t="s">
+      <c r="M12" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="N12" s="10" t="s">
+      <c r="N12" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="O12" s="10">
+      <c r="O12" s="9">
         <v>43007</v>
       </c>
-      <c r="P12" s="10" t="s">
+      <c r="P12" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="Q12" s="10" t="s">
+      <c r="Q12" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R12" s="10" t="s">
+      <c r="R12" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S12" s="11"/>
     </row>
-    <row r="13" spans="1:19" ht="60">
-      <c r="A13" s="10" t="s">
+    <row r="13" spans="1:19" ht="64">
+      <c r="A13" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="H13" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="I13" s="9" t="s">
         <v>131</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="J13" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="K13" s="10" t="s">
+      <c r="K13" s="9" t="s">
         <v>133</v>
       </c>
-      <c r="L13" s="10" t="s">
+      <c r="L13" s="9" t="s">
         <v>134</v>
       </c>
-      <c r="M13" s="10" t="s">
+      <c r="M13" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="N13" s="10" t="s">
+      <c r="N13" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="O13" s="10">
+      <c r="O13" s="9">
         <v>43009</v>
       </c>
-      <c r="P13" s="10" t="s">
+      <c r="P13" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="Q13" s="10" t="s">
+      <c r="Q13" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R13" s="10" t="s">
+      <c r="R13" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S13" s="11"/>
     </row>
     <row r="14" spans="1:19">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="H14" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="I14" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="J14" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="K14" s="9" t="s">
         <v>142</v>
       </c>
-      <c r="L14" s="10" t="s">
+      <c r="L14" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="M14" s="10" t="s">
+      <c r="M14" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="N14" s="10" t="s">
+      <c r="N14" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="O14" s="10">
+      <c r="O14" s="9">
         <v>44140</v>
       </c>
-      <c r="P14" s="10" t="s">
+      <c r="P14" s="9" t="s">
         <v>285</v>
       </c>
-      <c r="Q14" s="10" t="s">
+      <c r="Q14" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R14" s="10" t="s">
+      <c r="R14" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S14" s="11"/>
     </row>
     <row r="15" spans="1:19">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="K15" s="10" t="s">
+      <c r="K15" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="L15" s="10" t="s">
+      <c r="L15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="M15" s="10" t="s">
+      <c r="M15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="N15" s="10" t="s">
+      <c r="N15" s="9" t="s">
         <v>286</v>
       </c>
-      <c r="O15" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="P15" s="10" t="s">
+      <c r="O15" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P15" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="Q15" s="10" t="s">
+      <c r="Q15" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R15" s="10" t="s">
+      <c r="R15" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S15" s="11"/>
     </row>
     <row r="16" spans="1:19">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>148</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="10" t="s">
+      <c r="C16" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="H16" s="10" t="s">
+      <c r="H16" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I16" s="10" t="s">
+      <c r="I16" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="J16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K16" s="10" t="s">
+      <c r="K16" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="L16" s="10" t="s">
+      <c r="L16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="M16" s="10" t="s">
+      <c r="M16" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="N16" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" s="10">
+      <c r="N16" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O16" s="9">
         <v>43851</v>
       </c>
-      <c r="P16" s="10" t="s">
+      <c r="P16" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="Q16" s="10" t="s">
+      <c r="Q16" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R16" s="10" t="s">
+      <c r="R16" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S16" s="11"/>
     </row>
     <row r="17" spans="1:19">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="J17" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="K17" s="10" t="s">
+      <c r="K17" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="L17" s="10" t="s">
+      <c r="L17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="M17" s="10" t="s">
+      <c r="M17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="N17" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="O17" s="10">
+      <c r="N17" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O17" s="9">
         <v>43897</v>
       </c>
-      <c r="P17" s="10" t="s">
+      <c r="P17" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="Q17" s="10" t="s">
+      <c r="Q17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R17" s="10" t="s">
+      <c r="R17" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S17" s="11"/>
     </row>
-    <row r="18" spans="1:19" ht="30">
-      <c r="A18" s="10" t="s">
+    <row r="18" spans="1:19" ht="32">
+      <c r="A18" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="C18" s="10" t="s">
+      <c r="C18" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="D18" s="10" t="s">
+      <c r="D18" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="E18" s="10" t="s">
+      <c r="E18" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="H18" s="10" t="s">
+      <c r="H18" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="I18" s="10" t="s">
+      <c r="I18" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="J18" s="10" t="s">
+      <c r="J18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="K18" s="10" t="s">
+      <c r="K18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="L18" s="10" t="s">
+      <c r="L18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="M18" s="10" t="s">
+      <c r="M18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="N18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="O18" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="P18" s="10" t="s">
+      <c r="N18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="O18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="P18" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="Q18" s="10" t="s">
+      <c r="Q18" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="R18" s="10" t="s">
+      <c r="R18" s="9" t="s">
         <v>64</v>
       </c>
       <c r="S18" s="11"/>
     </row>
-    <row r="19" spans="1:19" ht="31.5">
-      <c r="A19" s="19" t="s">
+    <row r="19" spans="1:19" ht="31">
+      <c r="A19" s="12" t="s">
         <v>194</v>
       </c>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="13" t="s">
         <v>195</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="12" t="s">
         <v>196</v>
       </c>
-      <c r="D19" s="19" t="s">
+      <c r="D19" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="F19" s="19" t="s">
+      <c r="F19" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="G19" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="H19" s="19" t="s">
+      <c r="G19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H19" s="12" t="s">
         <v>200</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="13" t="s">
         <v>201</v>
       </c>
-      <c r="J19" s="19" t="s">
+      <c r="J19" s="12" t="s">
         <v>202</v>
       </c>
-      <c r="K19" s="19" t="s">
+      <c r="K19" s="12" t="s">
         <v>203</v>
       </c>
-      <c r="L19" s="21" t="s">
+      <c r="L19" s="14" t="s">
         <v>204</v>
       </c>
-      <c r="M19" s="19" t="s">
+      <c r="M19" s="12" t="s">
         <v>205</v>
       </c>
-      <c r="N19" s="19" t="s">
-        <v>26</v>
-      </c>
-      <c r="O19" s="22">
+      <c r="N19" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="O19" s="15">
         <v>45258</v>
       </c>
-      <c r="P19" s="19" t="s">
+      <c r="P19" s="12" t="s">
         <v>206</v>
       </c>
-      <c r="Q19" s="19" t="s">
+      <c r="Q19" s="12" t="s">
         <v>207</v>
       </c>
-      <c r="R19" s="19" t="s">
+      <c r="R19" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="S19" s="23" t="s">
+      <c r="S19" s="16" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="31.5">
-      <c r="A20" s="26" t="s">
+    <row r="20" spans="1:19" ht="31">
+      <c r="A20" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="17" t="s">
         <v>292</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="17" t="s">
         <v>212</v>
       </c>
-      <c r="D20" s="26" t="s">
+      <c r="D20" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="17" t="s">
         <v>293</v>
       </c>
-      <c r="F20" s="27" t="s">
+      <c r="F20" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G20" s="26"/>
-      <c r="H20" s="27" t="s">
+      <c r="G20" s="17"/>
+      <c r="H20" s="17" t="s">
         <v>294</v>
       </c>
-      <c r="I20" s="27" t="s">
+      <c r="I20" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="J20" s="27" t="s">
+      <c r="J20" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="K20" s="28" t="s">
+      <c r="K20" s="18" t="s">
         <v>297</v>
       </c>
-      <c r="L20" s="26"/>
-      <c r="M20" s="27" t="s">
+      <c r="L20" s="17"/>
+      <c r="M20" s="17" t="s">
         <v>298</v>
       </c>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="27" t="s">
+      <c r="N20" s="17"/>
+      <c r="O20" s="17"/>
+      <c r="P20" s="17"/>
+      <c r="Q20" s="17"/>
+      <c r="R20" s="17" t="s">
         <v>299</v>
       </c>
-      <c r="S20" s="31" t="s">
+      <c r="S20" s="19" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="21" spans="1:19">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="D21" s="26" t="s">
+      <c r="D21" s="17" t="s">
         <v>137</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="17" t="s">
         <v>138</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F21" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="G21" s="27" t="s">
+      <c r="G21" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="27" t="s">
+      <c r="H21" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="I21" s="27" t="s">
+      <c r="I21" s="17" t="s">
         <v>301</v>
       </c>
-      <c r="J21" s="27" t="s">
+      <c r="J21" s="17" t="s">
         <v>302</v>
       </c>
-      <c r="K21" s="29" t="s">
+      <c r="K21" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="L21" s="26"/>
-      <c r="M21" s="27" t="s">
+      <c r="L21" s="17"/>
+      <c r="M21" s="17" t="s">
         <v>303</v>
       </c>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="27" t="s">
+      <c r="N21" s="17"/>
+      <c r="O21" s="17"/>
+      <c r="P21" s="17"/>
+      <c r="Q21" s="17"/>
+      <c r="R21" s="17" t="s">
         <v>299</v>
       </c>
-      <c r="S21" s="32"/>
+      <c r="S21" s="21"/>
     </row>
     <row r="22" spans="1:19">
-      <c r="A22" s="26" t="s">
+      <c r="A22" s="17" t="s">
         <v>216</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="22" t="s">
         <v>217</v>
       </c>
-      <c r="C22" s="26"/>
-      <c r="D22" s="27" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="17" t="s">
         <v>305</v>
       </c>
-      <c r="F22" s="27" t="s">
+      <c r="F22" s="17" t="s">
         <v>306</v>
       </c>
-      <c r="G22" s="26"/>
-      <c r="H22" s="27" t="s">
+      <c r="G22" s="17"/>
+      <c r="H22" s="17" t="s">
         <v>307</v>
       </c>
-      <c r="I22" s="27" t="s">
+      <c r="I22" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="J22" s="27" t="s">
+      <c r="J22" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="K22" s="27" t="s">
+      <c r="K22" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
-      <c r="Q22" s="26"/>
-      <c r="R22" s="27" t="s">
+      <c r="L22" s="17"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="17"/>
+      <c r="O22" s="17"/>
+      <c r="P22" s="17"/>
+      <c r="Q22" s="17"/>
+      <c r="R22" s="17" t="s">
         <v>299</v>
       </c>
-      <c r="S22" s="32"/>
-    </row>
-    <row r="23" spans="1:19" ht="31.5">
-      <c r="A23" s="40" t="s">
+      <c r="S22" s="21"/>
+    </row>
+    <row r="23" spans="1:19" ht="31">
+      <c r="A23" s="23" t="s">
         <v>219</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="42" t="s">
+      <c r="C23" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="D23" s="43" t="s">
+      <c r="D23" s="26" t="s">
         <v>221</v>
       </c>
-      <c r="E23" s="43" t="s">
+      <c r="E23" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="F23" s="44" t="s">
+      <c r="F23" s="27" t="s">
         <v>222</v>
       </c>
-      <c r="G23" s="45" t="s">
+      <c r="G23" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="H23" s="46" t="s">
+      <c r="H23" s="29" t="s">
         <v>224</v>
       </c>
-      <c r="I23" s="47" t="s">
+      <c r="I23" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="J23" s="48" t="s">
+      <c r="J23" s="30" t="s">
         <v>225</v>
       </c>
-      <c r="K23" s="49" t="s">
+      <c r="K23" s="31" t="s">
         <v>226</v>
       </c>
-      <c r="L23" s="47" t="s">
+      <c r="L23" s="23" t="s">
         <v>227</v>
       </c>
-      <c r="M23" s="47" t="s">
+      <c r="M23" s="23" t="s">
         <v>228</v>
       </c>
-      <c r="N23" s="40"/>
-      <c r="O23" s="40"/>
-      <c r="P23" s="47" t="s">
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23" t="s">
         <v>229</v>
       </c>
-      <c r="Q23" s="40"/>
-      <c r="R23" s="40"/>
-      <c r="S23" s="50" t="s">
+      <c r="Q23" s="23"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="32" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="24" spans="1:19">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="23" t="s">
         <v>230</v>
       </c>
-      <c r="B24" s="51" t="s">
+      <c r="B24" s="33" t="s">
         <v>231</v>
       </c>
-      <c r="C24" s="51" t="s">
+      <c r="C24" s="33" t="s">
         <v>232</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="31" t="s">
         <v>232</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="F24" s="27" t="s">
         <v>233</v>
       </c>
-      <c r="G24" s="47" t="s">
+      <c r="G24" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="H24" s="46" t="s">
+      <c r="H24" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="I24" s="47" t="s">
+      <c r="I24" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="J24" s="47" t="s">
+      <c r="J24" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="K24" s="49" t="s">
+      <c r="K24" s="31" t="s">
         <v>238</v>
       </c>
-      <c r="L24" s="47" t="s">
+      <c r="L24" s="23" t="s">
         <v>239</v>
       </c>
-      <c r="M24" s="40"/>
-      <c r="N24" s="52" t="s">
+      <c r="M24" s="23"/>
+      <c r="N24" s="34" t="s">
         <v>240</v>
       </c>
-      <c r="O24" s="40"/>
-      <c r="P24" s="47" t="s">
+      <c r="O24" s="23"/>
+      <c r="P24" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="Q24" s="47" t="s">
+      <c r="Q24" s="23" t="s">
         <v>242</v>
       </c>
-      <c r="R24" s="40"/>
-      <c r="S24" s="53"/>
-    </row>
-    <row r="25" spans="1:19" ht="31.5">
-      <c r="A25" s="33" t="s">
+      <c r="R24" s="23"/>
+      <c r="S24" s="35"/>
+    </row>
+    <row r="25" spans="1:19" ht="31">
+      <c r="A25" s="36" t="s">
         <v>243</v>
       </c>
-      <c r="B25" s="33" t="s">
+      <c r="B25" s="36" t="s">
         <v>244</v>
       </c>
-      <c r="C25" s="33" t="s">
+      <c r="C25" s="36" t="s">
         <v>245</v>
       </c>
-      <c r="D25" s="33" t="s">
+      <c r="D25" s="36" t="s">
         <v>245</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="F25" s="33" t="s">
+      <c r="F25" s="36" t="s">
         <v>246</v>
       </c>
-      <c r="G25" s="33" t="s">
+      <c r="G25" s="36" t="s">
         <v>247</v>
       </c>
-      <c r="H25" s="33" t="s">
+      <c r="H25" s="36" t="s">
         <v>248</v>
       </c>
-      <c r="I25" s="33" t="s">
+      <c r="I25" s="36" t="s">
         <v>249</v>
       </c>
-      <c r="J25" s="33" t="s">
+      <c r="J25" s="36" t="s">
         <v>250</v>
       </c>
-      <c r="K25" s="33" t="s">
+      <c r="K25" s="36" t="s">
         <v>251</v>
       </c>
-      <c r="L25" s="33" t="s">
+      <c r="L25" s="36" t="s">
         <v>252</v>
       </c>
-      <c r="M25" s="33" t="s">
+      <c r="M25" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="N25" s="33" t="s">
+      <c r="N25" s="36" t="s">
         <v>254</v>
       </c>
-      <c r="O25" s="34">
+      <c r="O25" s="37">
         <v>45224</v>
       </c>
-      <c r="P25" s="33" t="s">
+      <c r="P25" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="Q25" s="33" t="s">
+      <c r="Q25" s="36" t="s">
         <v>255</v>
       </c>
-      <c r="R25" s="33" t="s">
+      <c r="R25" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="S25" s="39" t="s">
+      <c r="S25" s="38" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="26" spans="1:19">
-      <c r="A26" s="35" t="s">
+      <c r="A26" s="36" t="s">
         <v>216</v>
       </c>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="36" t="s">
         <v>217</v>
       </c>
-      <c r="C26" s="33" t="s">
+      <c r="C26" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="D26" s="33" t="s">
+      <c r="D26" s="36" t="s">
         <v>257</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="F26" s="33" t="s">
+      <c r="F26" s="36" t="s">
         <v>258</v>
       </c>
-      <c r="G26" s="33" t="s">
+      <c r="G26" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="H26" s="33" t="s">
+      <c r="H26" s="36" t="s">
         <v>259</v>
       </c>
-      <c r="I26" s="33" t="s">
+      <c r="I26" s="36" t="s">
         <v>260</v>
       </c>
-      <c r="J26" s="33" t="s">
+      <c r="J26" s="36" t="s">
         <v>261</v>
       </c>
-      <c r="K26" s="35" t="s">
+      <c r="K26" s="36" t="s">
         <v>262</v>
       </c>
-      <c r="L26" s="33" t="s">
+      <c r="L26" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="M26" s="35" t="s">
+      <c r="M26" s="36" t="s">
         <v>263</v>
       </c>
-      <c r="N26" s="33" t="s">
+      <c r="N26" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="O26" s="36">
+      <c r="O26" s="39">
         <v>43691</v>
       </c>
-      <c r="P26" s="33" t="s">
+      <c r="P26" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="Q26" s="33" t="s">
+      <c r="Q26" s="36" t="s">
         <v>265</v>
       </c>
-      <c r="R26" s="33" t="s">
+      <c r="R26" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="S26" s="38"/>
-    </row>
-    <row r="27" spans="1:19" ht="51">
-      <c r="A27" s="35" t="s">
+      <c r="S26" s="40"/>
+    </row>
+    <row r="27" spans="1:19" ht="60">
+      <c r="A27" s="36" t="s">
         <v>266</v>
       </c>
-      <c r="B27" s="35" t="s">
+      <c r="B27" s="36" t="s">
         <v>267</v>
       </c>
-      <c r="C27" s="35" t="s">
+      <c r="C27" s="36" t="s">
         <v>268</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="D27" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="36" t="s">
         <v>86</v>
       </c>
-      <c r="F27" s="33" t="s">
+      <c r="F27" s="36" t="s">
         <v>269</v>
       </c>
-      <c r="G27" s="37" t="s">
+      <c r="G27" s="41" t="s">
         <v>270</v>
       </c>
-      <c r="H27" s="37" t="s">
+      <c r="H27" s="41" t="s">
         <v>271</v>
       </c>
-      <c r="I27" s="33" t="s">
+      <c r="I27" s="36" t="s">
         <v>272</v>
       </c>
-      <c r="J27" s="33" t="s">
+      <c r="J27" s="36" t="s">
         <v>273</v>
       </c>
-      <c r="K27" s="35" t="s">
+      <c r="K27" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="L27" s="35" t="s">
+      <c r="L27" s="36" t="s">
         <v>274</v>
       </c>
-      <c r="M27" s="35" t="s">
+      <c r="M27" s="36" t="s">
         <v>253</v>
       </c>
-      <c r="N27" s="35" t="s">
+      <c r="N27" s="36" t="s">
         <v>275</v>
       </c>
-      <c r="O27" s="36">
+      <c r="O27" s="39">
         <v>45232</v>
       </c>
-      <c r="P27" s="35" t="s">
+      <c r="P27" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="Q27" s="33" t="s">
+      <c r="Q27" s="36" t="s">
         <v>276</v>
       </c>
-      <c r="R27" s="33" t="s">
+      <c r="R27" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="S27" s="38"/>
-    </row>
-    <row r="28" spans="1:19" ht="31.5">
-      <c r="A28" s="54" t="s">
+      <c r="S27" s="40"/>
+    </row>
+    <row r="28" spans="1:19" ht="31">
+      <c r="A28" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="43" t="s">
         <v>314</v>
       </c>
-      <c r="C28" s="54" t="s">
+      <c r="C28" s="42" t="s">
         <v>315</v>
       </c>
-      <c r="D28" s="54" t="s">
+      <c r="D28" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="E28" s="54" t="s">
+      <c r="E28" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="F28" s="54" t="s">
+      <c r="F28" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="G28" s="56" t="s">
+      <c r="G28" s="44" t="s">
         <v>316</v>
       </c>
-      <c r="H28" s="56" t="s">
+      <c r="H28" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="I28" s="54" t="s">
+      <c r="I28" s="42" t="s">
         <v>317</v>
       </c>
-      <c r="J28" s="54" t="s">
+      <c r="J28" s="42" t="s">
         <v>318</v>
       </c>
-      <c r="K28" s="57" t="s">
+      <c r="K28" s="45" t="s">
         <v>319</v>
       </c>
-      <c r="L28" s="54" t="s">
+      <c r="L28" s="42" t="s">
         <v>320</v>
       </c>
-      <c r="M28" s="54" t="s">
+      <c r="M28" s="42" t="s">
         <v>321</v>
       </c>
-      <c r="N28" s="54" t="s">
+      <c r="N28" s="42" t="s">
         <v>320</v>
       </c>
-      <c r="O28" s="58">
+      <c r="O28" s="46">
         <v>43552</v>
       </c>
-      <c r="P28" s="54" t="s">
+      <c r="P28" s="42" t="s">
         <v>322</v>
       </c>
-      <c r="Q28" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="R28" s="56" t="s">
+      <c r="Q28" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="R28" s="44" t="s">
         <v>323</v>
       </c>
-      <c r="S28" s="59" t="s">
+      <c r="S28" s="47" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="29" spans="1:19">
-      <c r="A29" s="54" t="s">
+      <c r="A29" s="42" t="s">
         <v>324</v>
       </c>
-      <c r="B29" s="54" t="s">
+      <c r="B29" s="42" t="s">
         <v>325</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="C29" s="42" t="s">
         <v>326</v>
       </c>
-      <c r="D29" s="54" t="s">
+      <c r="D29" s="42" t="s">
         <v>327</v>
       </c>
-      <c r="E29" s="54" t="s">
+      <c r="E29" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="F29" s="54" t="s">
+      <c r="F29" s="42" t="s">
         <v>328</v>
       </c>
-      <c r="G29" s="54" t="s">
+      <c r="G29" s="42" t="s">
         <v>320</v>
       </c>
-      <c r="H29" s="56" t="s">
+      <c r="H29" s="44" t="s">
         <v>329</v>
       </c>
-      <c r="I29" s="54" t="s">
+      <c r="I29" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="J29" s="54" t="s">
+      <c r="J29" s="42" t="s">
         <v>330</v>
       </c>
-      <c r="K29" s="57" t="s">
+      <c r="K29" s="45" t="s">
         <v>331</v>
       </c>
-      <c r="L29" s="54" t="s">
+      <c r="L29" s="42" t="s">
         <v>320</v>
       </c>
-      <c r="M29" s="54" t="s">
+      <c r="M29" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="N29" s="54" t="s">
+      <c r="N29" s="42" t="s">
         <v>332</v>
       </c>
-      <c r="O29" s="58">
+      <c r="O29" s="46">
         <v>45050</v>
       </c>
-      <c r="P29" s="54" t="s">
+      <c r="P29" s="42" t="s">
         <v>333</v>
       </c>
-      <c r="Q29" s="54" t="s">
-        <v>26</v>
-      </c>
-      <c r="R29" s="56" t="s">
+      <c r="Q29" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="R29" s="44" t="s">
         <v>323</v>
       </c>
-      <c r="S29" s="60"/>
-    </row>
-    <row r="70" spans="1:4" ht="17.25">
-      <c r="B70" s="2" t="s">
+      <c r="S29" s="48"/>
+    </row>
+    <row r="70" spans="1:4" ht="17">
+      <c r="B70" s="49" t="s">
         <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:4">
-      <c r="B71" s="12" t="s">
+      <c r="B71" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="C71" s="13" t="s">
+      <c r="C71" s="51" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3469,94 +3482,94 @@
       <c r="B72" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="C72" s="14"/>
+      <c r="C72" s="52"/>
     </row>
     <row r="73" spans="1:4">
       <c r="B73" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="C73" s="14"/>
+      <c r="C73" s="52"/>
     </row>
     <row r="74" spans="1:4">
       <c r="B74" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="C74" s="14"/>
+      <c r="C74" s="52"/>
     </row>
     <row r="75" spans="1:4">
       <c r="B75" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C75" s="14"/>
+      <c r="C75" s="52"/>
     </row>
     <row r="76" spans="1:4">
       <c r="B76" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C76" s="14"/>
+      <c r="C76" s="52"/>
     </row>
     <row r="77" spans="1:4">
       <c r="B77" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="C77" s="14"/>
+      <c r="C77" s="52"/>
     </row>
     <row r="78" spans="1:4">
       <c r="B78" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="C78" s="14"/>
-    </row>
-    <row r="79" spans="1:4" ht="17.25">
-      <c r="A79" s="2" t="s">
+      <c r="C78" s="52"/>
+    </row>
+    <row r="79" spans="1:4" ht="17">
+      <c r="A79" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="B79" s="2" t="s">
+      <c r="B79" s="53" t="s">
         <v>173</v>
       </c>
-      <c r="C79" s="2" t="s">
+      <c r="C79" s="53" t="s">
         <v>174</v>
       </c>
-      <c r="D79" s="2" t="s">
+      <c r="D79" s="49" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="16.5">
-      <c r="A80" s="12" t="s">
+    <row r="80" spans="1:4" ht="17">
+      <c r="A80" s="50" t="s">
         <v>176</v>
       </c>
-      <c r="B80" s="15" t="s">
+      <c r="B80" s="54" t="s">
         <v>177</v>
       </c>
-      <c r="C80" s="12" t="s">
+      <c r="C80" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="D80" s="16" t="s">
+      <c r="D80" s="55" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="18">
-      <c r="A81" s="12" t="s">
+      <c r="A81" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="B81" s="17" t="s">
+      <c r="B81" s="56" t="s">
         <v>178</v>
       </c>
-      <c r="C81" s="12" t="s">
+      <c r="C81" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="D81" s="12" t="s">
+      <c r="D81" s="50" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="18">
-      <c r="A82" s="12" t="s">
+      <c r="A82" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="B82" s="17" t="s">
+      <c r="B82" s="56" t="s">
         <v>181</v>
       </c>
-      <c r="C82" s="12" t="s">
+      <c r="C82" s="50" t="s">
         <v>182</v>
       </c>
       <c r="D82" s="11" t="s">
@@ -3564,13 +3577,13 @@
       </c>
     </row>
     <row r="83" spans="1:4">
-      <c r="A83" s="12" t="s">
+      <c r="A83" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="B83" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C83" s="12" t="s">
+      <c r="B83" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C83" s="50" t="s">
         <v>184</v>
       </c>
       <c r="D83" s="11" t="s">
@@ -3578,13 +3591,13 @@
       </c>
     </row>
     <row r="84" spans="1:4">
-      <c r="A84" s="12" t="s">
+      <c r="A84" s="50" t="s">
         <v>185</v>
       </c>
-      <c r="B84" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C84" s="12" t="s">
+      <c r="B84" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C84" s="50" t="s">
         <v>182</v>
       </c>
       <c r="D84" s="11" t="s">
@@ -3592,13 +3605,13 @@
       </c>
     </row>
     <row r="85" spans="1:4">
-      <c r="A85" s="12" t="s">
+      <c r="A85" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="B85" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C85" s="12" t="s">
+      <c r="B85" s="57" t="s">
+        <v>26</v>
+      </c>
+      <c r="C85" s="50" t="s">
         <v>182</v>
       </c>
       <c r="D85" s="11" t="s">
@@ -3606,10 +3619,10 @@
       </c>
     </row>
     <row r="86" spans="1:4">
-      <c r="A86" s="12" t="s">
+      <c r="A86" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="B86" s="18" t="s">
+      <c r="B86" s="57" t="s">
         <v>26</v>
       </c>
       <c r="C86" s="11" t="s">
@@ -3620,10 +3633,10 @@
       </c>
     </row>
     <row r="87" spans="1:4">
-      <c r="A87" s="12" t="s">
+      <c r="A87" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="B87" s="18" t="s">
+      <c r="B87" s="57" t="s">
         <v>26</v>
       </c>
       <c r="C87" s="11" t="s">
@@ -3634,10 +3647,10 @@
       </c>
     </row>
     <row r="88" spans="1:4">
-      <c r="A88" s="12" t="s">
+      <c r="A88" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="B88" s="18" t="s">
+      <c r="B88" s="57" t="s">
         <v>26</v>
       </c>
       <c r="C88" s="11" t="s">
@@ -3648,10 +3661,10 @@
       </c>
     </row>
     <row r="89" spans="1:4">
-      <c r="A89" s="12" t="s">
+      <c r="A89" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="B89" s="18" t="s">
+      <c r="B89" s="57" t="s">
         <v>26</v>
       </c>
       <c r="C89" s="11" t="s">
@@ -3662,16 +3675,16 @@
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="3" t="s">
+      <c r="A90" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="B90" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C90" s="3" t="s">
+      <c r="B90" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="C90" s="58" t="s">
         <v>210</v>
       </c>
-      <c r="D90" s="3" t="s">
+      <c r="D90" s="58" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[group_results/Comparative_Analysis_of_IPs.xlsl] Solve Active since field type problem.
</commit_message>
<xml_diff>
--- a/manual/group_results/Comparative_Analysis_of_IPs.xlsx
+++ b/manual/group_results/Comparative_Analysis_of_IPs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/attrup/Desktop/University/Master/Cyber1/Project - Let Me Out/let-me-out/manual/group_results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gergelysalomvari/Documents/CYBER - AAU CPH/LetMeOut/let-me-out/manual/group_results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF05FF32-517F-C346-B821-F162DAE02FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8C71A6-1238-1D47-99ED-B507A34517CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16520" xr2:uid="{D0933BE7-A6D3-5840-9958-232435785B00}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28720" windowHeight="16520" xr2:uid="{D0933BE7-A6D3-5840-9958-232435785B00}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1165,6 +1165,7 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1412,7 +1413,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1482,18 +1483,21 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="5" fillId="9" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="9" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1821,8 +1825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2AB11E9-4A0D-624C-B54C-38C9E6714153}">
   <dimension ref="A1:S90"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="C71" sqref="C71:C78"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="O17" sqref="O16:O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -2182,7 +2186,7 @@
       <c r="N6" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="O6" s="9">
+      <c r="O6" s="59">
         <v>45262</v>
       </c>
       <c r="P6" s="9" t="s">
@@ -2239,7 +2243,7 @@
       <c r="N7" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="O7" s="9">
+      <c r="O7" s="59">
         <v>43381</v>
       </c>
       <c r="P7" s="9" t="s">
@@ -2353,7 +2357,7 @@
       <c r="N9" s="9" t="s">
         <v>281</v>
       </c>
-      <c r="O9" s="9">
+      <c r="O9" s="59">
         <v>44769</v>
       </c>
       <c r="P9" s="9" t="s">
@@ -2410,7 +2414,7 @@
       <c r="N10" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="O10" s="9">
+      <c r="O10" s="59">
         <v>44641</v>
       </c>
       <c r="P10" s="9" t="s">
@@ -2467,7 +2471,7 @@
       <c r="N11" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="O11" s="9">
+      <c r="O11" s="59">
         <v>44444</v>
       </c>
       <c r="P11" s="9" t="s">
@@ -2524,7 +2528,7 @@
       <c r="N12" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="O12" s="9">
+      <c r="O12" s="59">
         <v>43007</v>
       </c>
       <c r="P12" s="9" t="s">
@@ -2581,7 +2585,7 @@
       <c r="N13" s="9" t="s">
         <v>284</v>
       </c>
-      <c r="O13" s="9">
+      <c r="O13" s="59">
         <v>43009</v>
       </c>
       <c r="P13" s="9" t="s">
@@ -2638,7 +2642,7 @@
       <c r="N14" s="9" t="s">
         <v>283</v>
       </c>
-      <c r="O14" s="9">
+      <c r="O14" s="59">
         <v>44140</v>
       </c>
       <c r="P14" s="9" t="s">
@@ -2752,7 +2756,7 @@
       <c r="N16" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="O16" s="9">
+      <c r="O16" s="59">
         <v>43851</v>
       </c>
       <c r="P16" s="9" t="s">
@@ -2809,7 +2813,7 @@
       <c r="N17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="O17" s="9">
+      <c r="O17" s="59">
         <v>43897</v>
       </c>
       <c r="P17" s="9" t="s">
@@ -3474,7 +3478,7 @@
       <c r="B71" s="50" t="s">
         <v>164</v>
       </c>
-      <c r="C71" s="51" t="s">
+      <c r="C71" s="57" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3482,52 +3486,52 @@
       <c r="B72" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="C72" s="52"/>
+      <c r="C72" s="58"/>
     </row>
     <row r="73" spans="1:4">
       <c r="B73" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="C73" s="52"/>
+      <c r="C73" s="58"/>
     </row>
     <row r="74" spans="1:4">
       <c r="B74" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="C74" s="52"/>
+      <c r="C74" s="58"/>
     </row>
     <row r="75" spans="1:4">
       <c r="B75" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C75" s="52"/>
+      <c r="C75" s="58"/>
     </row>
     <row r="76" spans="1:4">
       <c r="B76" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="C76" s="52"/>
+      <c r="C76" s="58"/>
     </row>
     <row r="77" spans="1:4">
       <c r="B77" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="C77" s="52"/>
+      <c r="C77" s="58"/>
     </row>
     <row r="78" spans="1:4">
       <c r="B78" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="C78" s="52"/>
+      <c r="C78" s="58"/>
     </row>
     <row r="79" spans="1:4" ht="17">
       <c r="A79" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="B79" s="53" t="s">
+      <c r="B79" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="C79" s="53" t="s">
+      <c r="C79" s="51" t="s">
         <v>174</v>
       </c>
       <c r="D79" s="49" t="s">
@@ -3538,13 +3542,13 @@
       <c r="A80" s="50" t="s">
         <v>176</v>
       </c>
-      <c r="B80" s="54" t="s">
+      <c r="B80" s="52" t="s">
         <v>177</v>
       </c>
       <c r="C80" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="D80" s="55" t="s">
+      <c r="D80" s="53" t="s">
         <v>148</v>
       </c>
     </row>
@@ -3552,7 +3556,7 @@
       <c r="A81" s="50" t="s">
         <v>19</v>
       </c>
-      <c r="B81" s="56" t="s">
+      <c r="B81" s="54" t="s">
         <v>178</v>
       </c>
       <c r="C81" s="50" t="s">
@@ -3566,7 +3570,7 @@
       <c r="A82" s="50" t="s">
         <v>180</v>
       </c>
-      <c r="B82" s="56" t="s">
+      <c r="B82" s="54" t="s">
         <v>181</v>
       </c>
       <c r="C82" s="50" t="s">
@@ -3580,7 +3584,7 @@
       <c r="A83" s="50" t="s">
         <v>183</v>
       </c>
-      <c r="B83" s="57" t="s">
+      <c r="B83" s="55" t="s">
         <v>26</v>
       </c>
       <c r="C83" s="50" t="s">
@@ -3594,7 +3598,7 @@
       <c r="A84" s="50" t="s">
         <v>185</v>
       </c>
-      <c r="B84" s="57" t="s">
+      <c r="B84" s="55" t="s">
         <v>26</v>
       </c>
       <c r="C84" s="50" t="s">
@@ -3608,7 +3612,7 @@
       <c r="A85" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="B85" s="57" t="s">
+      <c r="B85" s="55" t="s">
         <v>26</v>
       </c>
       <c r="C85" s="50" t="s">
@@ -3622,7 +3626,7 @@
       <c r="A86" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="B86" s="57" t="s">
+      <c r="B86" s="55" t="s">
         <v>26</v>
       </c>
       <c r="C86" s="11" t="s">
@@ -3636,7 +3640,7 @@
       <c r="A87" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="B87" s="57" t="s">
+      <c r="B87" s="55" t="s">
         <v>26</v>
       </c>
       <c r="C87" s="11" t="s">
@@ -3650,7 +3654,7 @@
       <c r="A88" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="B88" s="57" t="s">
+      <c r="B88" s="55" t="s">
         <v>26</v>
       </c>
       <c r="C88" s="11" t="s">
@@ -3664,7 +3668,7 @@
       <c r="A89" s="50" t="s">
         <v>191</v>
       </c>
-      <c r="B89" s="57" t="s">
+      <c r="B89" s="55" t="s">
         <v>26</v>
       </c>
       <c r="C89" s="11" t="s">
@@ -3675,16 +3679,16 @@
       </c>
     </row>
     <row r="90" spans="1:4">
-      <c r="A90" s="58" t="s">
+      <c r="A90" s="56" t="s">
         <v>209</v>
       </c>
-      <c r="B90" s="58" t="s">
-        <v>26</v>
-      </c>
-      <c r="C90" s="58" t="s">
+      <c r="B90" s="56" t="s">
+        <v>26</v>
+      </c>
+      <c r="C90" s="56" t="s">
         <v>210</v>
       </c>
-      <c r="D90" s="58" t="s">
+      <c r="D90" s="56" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>